<commit_message>
Feature/fix trer66 (#85) 9a975a6f56d1e66dec72f3bc14a23df3162dd0d9
</commit_message>
<xml_diff>
--- a/main/ig/ValueSet-sas-valueset-categorieetablissement.xlsx
+++ b/main/ig/ValueSet-sas-valueset-categorieetablissement.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-06T14:17:39+00:00</t>
+    <t>2024-11-08T16:57:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>System URI</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/TRE_R66-CategorieEtablissement/TRE_R66-CategorieEtablissement</t>
+    <t>https://mos.esante.gouv.fr/NOS/TRE_R66-CategorieEtablissement/FHIR/TRE-R66-CategorieEtablissement</t>
   </si>
 </sst>
 </file>

</xml_diff>